<commit_message>
Download some papers, sort the xlsx and add more tools
</commit_message>
<xml_diff>
--- a/Android恶意软件检测工具.xlsx
+++ b/Android恶意软件检测工具.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="应用仓库" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="126">
   <si>
     <t>论文</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -34,32 +34,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>android恶意软件库</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>D. E. Krutz, et al., “A dataset of open-source Android applications,” in Proc. 12th Working Conf. Mining Softw. Repositories, 2015, pp. 522–525</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>开源应用数据集</t>
-  </si>
-  <si>
     <t>R. Stevens, J. Ganz, V. Filkov, P. Devanbu, and H. Chen, “Asking for (and about) permissions used by Android apps,” in Proc. 10th Working Conf. Mining Softw. Repositories, 2013, pp. 31–40.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>AndroZoo: apk数据集</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Y. Zhou and X. Jiang, “Dissecting Android Malware: Characterization and evolution,” in Proc. IEEE Symp. Secur. Privacy, 2012, pp. 95–109.</t>
-  </si>
-  <si>
-    <t>恶意软件仓库 第二个需翻墙</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">https://virusshare.com/ </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -73,10 +55,6 @@
   </si>
   <si>
     <t>PlayDrone: Google Play  爬虫</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>爬虫</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -412,18 +390,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>http://www.malgenomeproject.org</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>android恶意软件库(1000+)，但是目前已经弃项了。（不过曾向南大公布过datasets，求助陈老师）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https//www.sec.cs.tu-bs.de/~danarp/drebin/index.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>android恶意软件库（5000+）10~12年的，高校教职人员可以发送邮件获取，并且向南大开放</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -432,6 +398,85 @@
   </si>
   <si>
     <t>通过APP的Dalvik字节码进行静态检测，主要检测APP中潜在的恶意行为，会自动生成txt或html格式的报告</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>状态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>备注</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://github.com/AndroSec/AndroSecDatabases</t>
+  </si>
+  <si>
+    <t>开源应用数据集，包含1179个引用，4416个版本和435680的提交，以及使用Androguard，Sonar和Stowaway；以及清单文件/权限的分析。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Daniel Arp, Michael Spreitzenbarth, Malte Huebner, Hugo Gascon, and Konrad Rieck "Drebin: Efficient and Explainable Detection of Android Malware in Your Pocket", 21th Annual Network and Distributed System Security Symposium (NDSS), </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AndroZoo: Apk数据集</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://blog.csdn.net/u013107656/article/details/67632235</t>
+  </si>
+  <si>
+    <t>移动应用安全工具总结，谁来整合一下</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://androzoo.uni.lu/apklyze/</t>
+  </si>
+  <si>
+    <t>AndroidZoo的分析工具</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>请房老师发邮件要数据，具体请参见：https://androzoo.uni.lu/access</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>目前已经弃项，不过曾向南大公布过datasets，请房老师再看看有没有机会弄到数据库</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.malgenomeproject.org/android </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://androzoo.uni.lu/access</t>
+  </si>
+  <si>
+    <t>https://virusshare.com/research.4n6</t>
+  </si>
+  <si>
+    <t>提到了很多关于安卓恶意软件分析的论文</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>请房老师发邮件要数据，具体请参见：https://virusshare.com/about.4n6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.sec.cs.tu-bs.de/~danarp/drebin/index.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>请房老师发邮件要数据，具体请参见：https://www.sec.cs.tu-bs.de/~danarp/drebin/index.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>正在拉取</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>android恶意软件库，恶意软件库(1000+)。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -524,19 +569,13 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -544,8 +583,18 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -553,7 +602,7 @@
     <cellStyle name="超链接" xfId="2" builtinId="8"/>
     <cellStyle name="计算" xfId="1" builtinId="22"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="10">
     <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -562,6 +611,15 @@
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -593,22 +651,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:B11" totalsRowShown="0" dataDxfId="6" tableBorderDxfId="5" headerRowCellStyle="常规">
-  <autoFilter ref="A1:B11"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="论文" dataDxfId="4"/>
-    <tableColumn id="2" name="描述" dataDxfId="3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:D11" totalsRowShown="0" dataDxfId="9" tableBorderDxfId="8" headerRowCellStyle="常规">
+  <autoFilter ref="A1:D11"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="论文" dataDxfId="7"/>
+    <tableColumn id="2" name="描述" dataDxfId="6"/>
+    <tableColumn id="3" name="状态" dataDxfId="5"/>
+    <tableColumn id="4" name="备注" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A1:B51" totalsRowShown="0" dataDxfId="2">
-  <autoFilter ref="A1:B51"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="论文" dataDxfId="1"/>
-    <tableColumn id="2" name="描述" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A1:C54" totalsRowShown="0" dataDxfId="3">
+  <autoFilter ref="A1:C54"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="论文" dataDxfId="2"/>
+    <tableColumn id="2" name="描述" dataDxfId="1"/>
+    <tableColumn id="3" name="状态" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -877,123 +938,162 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D14" sqref="D13:D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="61.88671875" customWidth="1"/>
-    <col min="2" max="2" width="53.88671875" customWidth="1"/>
+    <col min="1" max="1" width="47.77734375" customWidth="1"/>
+    <col min="2" max="2" width="39.33203125" customWidth="1"/>
+    <col min="3" max="3" width="40.109375" customWidth="1"/>
+    <col min="4" max="4" width="51.109375" customWidth="1"/>
+    <col min="5" max="5" width="44.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="C1" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="55.2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="55.2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C5" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" ht="69" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" ht="55.2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="3"/>
-    </row>
-    <row r="8" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>111</v>
-      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A10" r:id="rId1"/>
+    <hyperlink ref="A5" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="D6" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B53"/>
+  <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1002,402 +1102,479 @@
     <col min="2" max="2" width="62.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="C1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:3" ht="55.2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="6"/>
-    </row>
-    <row r="3" spans="1:2" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="55.2" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="B7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="B8" s="4"/>
+      <c r="C8" s="3"/>
+    </row>
+    <row r="9" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="B9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="C9" s="3"/>
+    </row>
+    <row r="10" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="B10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="C10" s="3"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="6"/>
-    </row>
-    <row r="9" spans="1:2" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="B12" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="C12" s="3"/>
+    </row>
+    <row r="13" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="B13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="C13" s="3"/>
+    </row>
+    <row r="14" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="B14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="5"/>
-    </row>
-    <row r="12" spans="1:2" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="C14" s="3"/>
+    </row>
+    <row r="15" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B15" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="C15" s="3"/>
+    </row>
+    <row r="16" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B16" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="C16" s="3"/>
+    </row>
+    <row r="17" spans="1:3" ht="55.2" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B17" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="C17" s="3"/>
+    </row>
+    <row r="18" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B18" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+      <c r="C18" s="3"/>
+    </row>
+    <row r="19" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B19" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="55.2" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="C19" s="3"/>
+    </row>
+    <row r="20" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B20" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B21" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+      <c r="C21" s="3"/>
+    </row>
+    <row r="22" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B22" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+      <c r="C22" s="3"/>
+    </row>
+    <row r="23" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B23" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+      <c r="C23" s="3"/>
+    </row>
+    <row r="24" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B24" s="3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+      <c r="C24" s="3"/>
+    </row>
+    <row r="25" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B25" s="3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+      <c r="C25" s="3"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B26" s="4"/>
+      <c r="C26" s="3"/>
+    </row>
+    <row r="27" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
+      <c r="B27" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="C27" s="3"/>
+    </row>
+    <row r="28" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+      <c r="B28" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="C28" s="3"/>
+    </row>
+    <row r="29" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+      <c r="B29" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B26" s="6"/>
-    </row>
-    <row r="27" spans="1:2" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
+      <c r="C29" s="3"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B30" s="4"/>
+      <c r="C30" s="3"/>
+    </row>
+    <row r="31" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
+      <c r="B31" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="C31" s="3"/>
+    </row>
+    <row r="32" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
+      <c r="B32" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="C32" s="3"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
+      <c r="B33" s="4"/>
+      <c r="C33" s="3"/>
+    </row>
+    <row r="34" spans="1:3" ht="55.2" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B30" s="6"/>
-    </row>
-    <row r="31" spans="1:2" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
+      <c r="B34" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C34" s="3"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B35" s="3" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
+      <c r="C35" s="3"/>
+    </row>
+    <row r="36" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B36" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
+      <c r="C36" s="3"/>
+    </row>
+    <row r="37" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B33" s="6"/>
-    </row>
-    <row r="34" spans="1:2" ht="55.2" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
+      <c r="B37" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B34" s="5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
+      <c r="C37" s="3"/>
+    </row>
+    <row r="38" spans="1:3" ht="55.2" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B38" s="3" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
+      <c r="C38" s="3"/>
+    </row>
+    <row r="39" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B39" s="3" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
+      <c r="C39" s="3"/>
+    </row>
+    <row r="40" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B40" s="3" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" ht="55.2" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
+      <c r="C40" s="3"/>
+    </row>
+    <row r="41" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B41" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
+      <c r="C41" s="3"/>
+    </row>
+    <row r="42" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B42" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="C42" s="3"/>
+    </row>
+    <row r="43" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A40" s="5" t="s">
+      <c r="B43" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="C43" s="3"/>
+    </row>
+    <row r="44" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
+      <c r="B44" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="C44" s="3"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="B42" s="5" t="s">
+      <c r="B45" s="4"/>
+      <c r="C45" s="3"/>
+    </row>
+    <row r="46" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
+      <c r="B46" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="C46" s="3"/>
+    </row>
+    <row r="47" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A44" s="5" t="s">
+      <c r="B47" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="C47" s="3"/>
+    </row>
+    <row r="48" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="6" t="s">
+      <c r="B48" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B45" s="6"/>
-    </row>
-    <row r="46" spans="1:2" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A46" s="5" t="s">
+      <c r="C48" s="3"/>
+    </row>
+    <row r="49" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B49" s="3" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
+      <c r="C49" s="3"/>
+    </row>
+    <row r="50" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B50" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A48" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A49" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A50" s="5" t="s">
+      <c r="C50" s="3"/>
+    </row>
+    <row r="51" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="B51" s="3" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A51" s="5" t="s">
+      <c r="C51" s="3"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B52" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B51" s="5" t="s">
+      <c r="C52" s="3"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B53" s="4"/>
+      <c r="B53" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C53" s="3"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C54" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
show a merging solution
</commit_message>
<xml_diff>
--- a/Android恶意软件检测工具.xlsx
+++ b/Android恶意软件检测工具.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="应用仓库" sheetId="1" r:id="rId1"/>
@@ -480,7 +480,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>testA</t>
+    <t>testB</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -944,20 +944,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.75" customWidth="1"/>
-    <col min="2" max="2" width="39.375" customWidth="1"/>
-    <col min="3" max="3" width="40.125" customWidth="1"/>
-    <col min="4" max="4" width="51.125" customWidth="1"/>
-    <col min="5" max="5" width="44.375" customWidth="1"/>
+    <col min="1" max="1" width="47.77734375" customWidth="1"/>
+    <col min="2" max="2" width="39.33203125" customWidth="1"/>
+    <col min="3" max="3" width="40.109375" customWidth="1"/>
+    <col min="4" max="4" width="51.109375" customWidth="1"/>
+    <col min="5" max="5" width="44.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -971,7 +971,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -985,7 +985,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="57" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -999,7 +999,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="57" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1013,7 +1013,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
@@ -1025,7 +1025,7 @@
       </c>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:4" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="69" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>109</v>
       </c>
@@ -1039,7 +1039,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -1051,7 +1051,7 @@
       </c>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:4" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1061,19 +1061,19 @@
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -1102,13 +1102,13 @@
       <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="65.375" customWidth="1"/>
-    <col min="2" max="2" width="62.125" customWidth="1"/>
+    <col min="1" max="1" width="65.33203125" customWidth="1"/>
+    <col min="2" max="2" width="62.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1119,14 +1119,14 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
@@ -1135,7 +1135,7 @@
       </c>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:3" ht="57" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
@@ -1144,7 +1144,7 @@
       </c>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
@@ -1153,7 +1153,7 @@
       </c>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
@@ -1162,7 +1162,7 @@
       </c>
       <c r="C6" s="3"/>
     </row>
-    <row r="7" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>19</v>
       </c>
@@ -1171,14 +1171,14 @@
       </c>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>22</v>
       </c>
@@ -1187,7 +1187,7 @@
       </c>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>24</v>
       </c>
@@ -1196,14 +1196,14 @@
       </c>
       <c r="C10" s="3"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
     </row>
-    <row r="12" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>27</v>
       </c>
@@ -1212,7 +1212,7 @@
       </c>
       <c r="C12" s="3"/>
     </row>
-    <row r="13" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>29</v>
       </c>
@@ -1221,7 +1221,7 @@
       </c>
       <c r="C13" s="3"/>
     </row>
-    <row r="14" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>31</v>
       </c>
@@ -1230,7 +1230,7 @@
       </c>
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>33</v>
       </c>
@@ -1239,7 +1239,7 @@
       </c>
       <c r="C15" s="3"/>
     </row>
-    <row r="16" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>35</v>
       </c>
@@ -1248,7 +1248,7 @@
       </c>
       <c r="C16" s="3"/>
     </row>
-    <row r="17" spans="1:3" ht="57" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>37</v>
       </c>
@@ -1257,7 +1257,7 @@
       </c>
       <c r="C17" s="3"/>
     </row>
-    <row r="18" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>39</v>
       </c>
@@ -1266,7 +1266,7 @@
       </c>
       <c r="C18" s="3"/>
     </row>
-    <row r="19" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>41</v>
       </c>
@@ -1275,7 +1275,7 @@
       </c>
       <c r="C19" s="3"/>
     </row>
-    <row r="20" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>43</v>
       </c>
@@ -1284,7 +1284,7 @@
       </c>
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>45</v>
       </c>
@@ -1293,7 +1293,7 @@
       </c>
       <c r="C21" s="3"/>
     </row>
-    <row r="22" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>47</v>
       </c>
@@ -1302,7 +1302,7 @@
       </c>
       <c r="C22" s="3"/>
     </row>
-    <row r="23" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>49</v>
       </c>
@@ -1311,7 +1311,7 @@
       </c>
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>51</v>
       </c>
@@ -1320,7 +1320,7 @@
       </c>
       <c r="C24" s="3"/>
     </row>
-    <row r="25" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>53</v>
       </c>
@@ -1329,14 +1329,14 @@
       </c>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>55</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="3"/>
     </row>
-    <row r="27" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>56</v>
       </c>
@@ -1345,7 +1345,7 @@
       </c>
       <c r="C27" s="3"/>
     </row>
-    <row r="28" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>58</v>
       </c>
@@ -1354,7 +1354,7 @@
       </c>
       <c r="C28" s="3"/>
     </row>
-    <row r="29" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>60</v>
       </c>
@@ -1363,14 +1363,14 @@
       </c>
       <c r="C29" s="3"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>62</v>
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="3"/>
     </row>
-    <row r="31" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>63</v>
       </c>
@@ -1379,7 +1379,7 @@
       </c>
       <c r="C31" s="3"/>
     </row>
-    <row r="32" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>65</v>
       </c>
@@ -1388,14 +1388,14 @@
       </c>
       <c r="C32" s="3"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>67</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="3"/>
     </row>
-    <row r="34" spans="1:3" ht="57" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>68</v>
       </c>
@@ -1404,7 +1404,7 @@
       </c>
       <c r="C34" s="3"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>69</v>
       </c>
@@ -1413,7 +1413,7 @@
       </c>
       <c r="C35" s="3"/>
     </row>
-    <row r="36" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>71</v>
       </c>
@@ -1422,7 +1422,7 @@
       </c>
       <c r="C36" s="3"/>
     </row>
-    <row r="37" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>73</v>
       </c>
@@ -1431,7 +1431,7 @@
       </c>
       <c r="C37" s="3"/>
     </row>
-    <row r="38" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>75</v>
       </c>
@@ -1440,7 +1440,7 @@
       </c>
       <c r="C38" s="3"/>
     </row>
-    <row r="39" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>77</v>
       </c>
@@ -1449,7 +1449,7 @@
       </c>
       <c r="C39" s="3"/>
     </row>
-    <row r="40" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>79</v>
       </c>
@@ -1458,7 +1458,7 @@
       </c>
       <c r="C40" s="3"/>
     </row>
-    <row r="41" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>81</v>
       </c>
@@ -1467,7 +1467,7 @@
       </c>
       <c r="C41" s="3"/>
     </row>
-    <row r="42" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>99</v>
       </c>
@@ -1476,7 +1476,7 @@
       </c>
       <c r="C42" s="3"/>
     </row>
-    <row r="43" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>84</v>
       </c>
@@ -1485,7 +1485,7 @@
       </c>
       <c r="C43" s="3"/>
     </row>
-    <row r="44" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>86</v>
       </c>
@@ -1494,14 +1494,14 @@
       </c>
       <c r="C44" s="3"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>88</v>
       </c>
       <c r="B45" s="4"/>
       <c r="C45" s="3"/>
     </row>
-    <row r="46" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>89</v>
       </c>
@@ -1510,7 +1510,7 @@
       </c>
       <c r="C46" s="3"/>
     </row>
-    <row r="47" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>91</v>
       </c>
@@ -1519,7 +1519,7 @@
       </c>
       <c r="C47" s="3"/>
     </row>
-    <row r="48" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>93</v>
       </c>
@@ -1528,7 +1528,7 @@
       </c>
       <c r="C48" s="3"/>
     </row>
-    <row r="49" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>95</v>
       </c>
@@ -1537,7 +1537,7 @@
       </c>
       <c r="C49" s="3"/>
     </row>
-    <row r="50" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>97</v>
       </c>
@@ -1546,7 +1546,7 @@
       </c>
       <c r="C50" s="3"/>
     </row>
-    <row r="51" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>103</v>
       </c>
@@ -1555,7 +1555,7 @@
       </c>
       <c r="C51" s="3"/>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>111</v>
       </c>
@@ -1564,7 +1564,7 @@
       </c>
       <c r="C52" s="3"/>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>113</v>
       </c>
@@ -1573,7 +1573,7 @@
       </c>
       <c r="C53" s="3"/>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>119</v>
       </c>

</xml_diff>

<commit_message>
fix the merging problem
</commit_message>
<xml_diff>
--- a/Android恶意软件检测工具.xlsx
+++ b/Android恶意软件检测工具.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="应用仓库" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="127">
   <si>
     <t>论文</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -477,6 +477,10 @@
   </si>
   <si>
     <t>android恶意软件库，恶意软件库(1000+)。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>aaa</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -941,19 +945,19 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="47.77734375" customWidth="1"/>
-    <col min="2" max="2" width="39.33203125" customWidth="1"/>
-    <col min="3" max="3" width="40.109375" customWidth="1"/>
-    <col min="4" max="4" width="51.109375" customWidth="1"/>
-    <col min="5" max="5" width="44.33203125" customWidth="1"/>
+    <col min="1" max="1" width="47.75" customWidth="1"/>
+    <col min="2" max="2" width="39.375" customWidth="1"/>
+    <col min="3" max="3" width="40.125" customWidth="1"/>
+    <col min="4" max="4" width="51.125" customWidth="1"/>
+    <col min="5" max="5" width="44.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -967,7 +971,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -981,7 +985,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -995,7 +999,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1009,7 +1013,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
@@ -1021,7 +1025,7 @@
       </c>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:4" ht="69" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>109</v>
       </c>
@@ -1035,17 +1039,19 @@
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>126</v>
+      </c>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:4" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1055,19 +1061,19 @@
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -1096,13 +1102,13 @@
       <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="65.33203125" customWidth="1"/>
-    <col min="2" max="2" width="62.109375" customWidth="1"/>
+    <col min="1" max="1" width="65.375" customWidth="1"/>
+    <col min="2" max="2" width="62.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1113,14 +1119,14 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
@@ -1129,7 +1135,7 @@
       </c>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:3" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="57" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
@@ -1138,7 +1144,7 @@
       </c>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
@@ -1147,7 +1153,7 @@
       </c>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
@@ -1156,7 +1162,7 @@
       </c>
       <c r="C6" s="3"/>
     </row>
-    <row r="7" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>19</v>
       </c>
@@ -1165,14 +1171,14 @@
       </c>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>22</v>
       </c>
@@ -1181,7 +1187,7 @@
       </c>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>24</v>
       </c>
@@ -1190,14 +1196,14 @@
       </c>
       <c r="C10" s="3"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
     </row>
-    <row r="12" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>27</v>
       </c>
@@ -1206,7 +1212,7 @@
       </c>
       <c r="C12" s="3"/>
     </row>
-    <row r="13" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>29</v>
       </c>
@@ -1215,7 +1221,7 @@
       </c>
       <c r="C13" s="3"/>
     </row>
-    <row r="14" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>31</v>
       </c>
@@ -1224,7 +1230,7 @@
       </c>
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>33</v>
       </c>
@@ -1233,7 +1239,7 @@
       </c>
       <c r="C15" s="3"/>
     </row>
-    <row r="16" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>35</v>
       </c>
@@ -1242,7 +1248,7 @@
       </c>
       <c r="C16" s="3"/>
     </row>
-    <row r="17" spans="1:3" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="57" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>37</v>
       </c>
@@ -1251,7 +1257,7 @@
       </c>
       <c r="C17" s="3"/>
     </row>
-    <row r="18" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>39</v>
       </c>
@@ -1260,7 +1266,7 @@
       </c>
       <c r="C18" s="3"/>
     </row>
-    <row r="19" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>41</v>
       </c>
@@ -1269,7 +1275,7 @@
       </c>
       <c r="C19" s="3"/>
     </row>
-    <row r="20" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>43</v>
       </c>
@@ -1278,7 +1284,7 @@
       </c>
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>45</v>
       </c>
@@ -1287,7 +1293,7 @@
       </c>
       <c r="C21" s="3"/>
     </row>
-    <row r="22" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>47</v>
       </c>
@@ -1296,7 +1302,7 @@
       </c>
       <c r="C22" s="3"/>
     </row>
-    <row r="23" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>49</v>
       </c>
@@ -1305,7 +1311,7 @@
       </c>
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>51</v>
       </c>
@@ -1314,7 +1320,7 @@
       </c>
       <c r="C24" s="3"/>
     </row>
-    <row r="25" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>53</v>
       </c>
@@ -1323,14 +1329,14 @@
       </c>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>55</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="3"/>
     </row>
-    <row r="27" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>56</v>
       </c>
@@ -1339,7 +1345,7 @@
       </c>
       <c r="C27" s="3"/>
     </row>
-    <row r="28" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>58</v>
       </c>
@@ -1348,7 +1354,7 @@
       </c>
       <c r="C28" s="3"/>
     </row>
-    <row r="29" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>60</v>
       </c>
@@ -1357,14 +1363,14 @@
       </c>
       <c r="C29" s="3"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>62</v>
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="3"/>
     </row>
-    <row r="31" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>63</v>
       </c>
@@ -1373,7 +1379,7 @@
       </c>
       <c r="C31" s="3"/>
     </row>
-    <row r="32" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>65</v>
       </c>
@@ -1382,14 +1388,14 @@
       </c>
       <c r="C32" s="3"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>67</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="3"/>
     </row>
-    <row r="34" spans="1:3" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" ht="57" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>68</v>
       </c>
@@ -1398,7 +1404,7 @@
       </c>
       <c r="C34" s="3"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>69</v>
       </c>
@@ -1407,7 +1413,7 @@
       </c>
       <c r="C35" s="3"/>
     </row>
-    <row r="36" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>71</v>
       </c>
@@ -1416,7 +1422,7 @@
       </c>
       <c r="C36" s="3"/>
     </row>
-    <row r="37" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>73</v>
       </c>
@@ -1425,7 +1431,7 @@
       </c>
       <c r="C37" s="3"/>
     </row>
-    <row r="38" spans="1:3" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>75</v>
       </c>
@@ -1434,7 +1440,7 @@
       </c>
       <c r="C38" s="3"/>
     </row>
-    <row r="39" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>77</v>
       </c>
@@ -1443,7 +1449,7 @@
       </c>
       <c r="C39" s="3"/>
     </row>
-    <row r="40" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>79</v>
       </c>
@@ -1452,7 +1458,7 @@
       </c>
       <c r="C40" s="3"/>
     </row>
-    <row r="41" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>81</v>
       </c>
@@ -1461,7 +1467,7 @@
       </c>
       <c r="C41" s="3"/>
     </row>
-    <row r="42" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>99</v>
       </c>
@@ -1470,7 +1476,7 @@
       </c>
       <c r="C42" s="3"/>
     </row>
-    <row r="43" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>84</v>
       </c>
@@ -1479,7 +1485,7 @@
       </c>
       <c r="C43" s="3"/>
     </row>
-    <row r="44" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>86</v>
       </c>
@@ -1488,14 +1494,14 @@
       </c>
       <c r="C44" s="3"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>88</v>
       </c>
       <c r="B45" s="4"/>
       <c r="C45" s="3"/>
     </row>
-    <row r="46" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>89</v>
       </c>
@@ -1504,7 +1510,7 @@
       </c>
       <c r="C46" s="3"/>
     </row>
-    <row r="47" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>91</v>
       </c>
@@ -1513,7 +1519,7 @@
       </c>
       <c r="C47" s="3"/>
     </row>
-    <row r="48" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>93</v>
       </c>
@@ -1522,7 +1528,7 @@
       </c>
       <c r="C48" s="3"/>
     </row>
-    <row r="49" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>95</v>
       </c>
@@ -1531,7 +1537,7 @@
       </c>
       <c r="C49" s="3"/>
     </row>
-    <row r="50" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>97</v>
       </c>
@@ -1540,7 +1546,7 @@
       </c>
       <c r="C50" s="3"/>
     </row>
-    <row r="51" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>103</v>
       </c>
@@ -1549,7 +1555,7 @@
       </c>
       <c r="C51" s="3"/>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>111</v>
       </c>
@@ -1558,7 +1564,7 @@
       </c>
       <c r="C52" s="3"/>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>113</v>
       </c>
@@ -1567,7 +1573,7 @@
       </c>
       <c r="C53" s="3"/>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>119</v>
       </c>

</xml_diff>